<commit_message>
Update degree architecture (MS-DIS)
</commit_message>
<xml_diff>
--- a/data/M1-MS-DIS.xlsx
+++ b/data/M1-MS-DIS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10905"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/olivier/SSDS/enseignement/UFR STAPS/Direction/Outils/celcatreport/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96FFEC90-FAFA-C94A-9D4B-60AEB4EF56C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8D5EAC7-68BF-BD48-B172-789371B8C408}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="780" windowWidth="34200" windowHeight="19720" xr2:uid="{154AE90F-D41B-8B49-BA91-D855BEB6F170}"/>
+    <workbookView xWindow="0" yWindow="700" windowWidth="34200" windowHeight="19700" xr2:uid="{154AE90F-D41B-8B49-BA91-D855BEB6F170}"/>
   </bookViews>
   <sheets>
     <sheet name="M1-MS-DIS" sheetId="1" r:id="rId1"/>
@@ -586,7 +586,7 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -843,7 +843,7 @@
         <v>4</v>
       </c>
       <c r="E9" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="F9" s="1">
         <v>12</v>

</xml_diff>